<commit_message>
Remove duplicated line in Excel file.
</commit_message>
<xml_diff>
--- a/Goals, Target, and Indicators.xlsx
+++ b/Goals, Target, and Indicators.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="645">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="645">
   <si>
     <t>Goal</t>
   </si>
@@ -3875,13 +3875,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E205"/>
+  <dimension ref="A1:E204"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D183" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="A205" sqref="A205"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3945,20 +3945,20 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="A6">
         <v>1</v>
       </c>
+      <c r="B6">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -3966,13 +3966,13 @@
         <v>1</v>
       </c>
       <c r="B7">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
@@ -3986,13 +3986,13 @@
         <v>1.2</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -4000,16 +4000,16 @@
         <v>1</v>
       </c>
       <c r="B9">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -4017,16 +4017,16 @@
         <v>1</v>
       </c>
       <c r="B10">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -4034,16 +4034,16 @@
         <v>1</v>
       </c>
       <c r="B11">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -4054,10 +4054,10 @@
         <v>1.5</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E12" t="s">
         <v>12</v>
@@ -4067,18 +4067,16 @@
       <c r="A13">
         <v>1</v>
       </c>
-      <c r="B13">
-        <v>1.5</v>
+      <c r="B13" t="s">
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" t="s">
-        <v>12</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="E13"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -4088,25 +4086,27 @@
         <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14"/>
+        <v>26</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s">
         <v>17</v>
@@ -4114,19 +4114,19 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
-        <v>27</v>
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>2.1</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E16" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -4137,10 +4137,10 @@
         <v>2.1</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E17" t="s">
         <v>7</v>
@@ -4151,13 +4151,13 @@
         <v>2</v>
       </c>
       <c r="B18">
-        <v>2.1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E18" t="s">
         <v>7</v>
@@ -4168,16 +4168,16 @@
         <v>2</v>
       </c>
       <c r="B19">
-        <v>2.2000000000000002</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E19" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -4188,10 +4188,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E20" t="s">
         <v>17</v>
@@ -4202,13 +4202,13 @@
         <v>2</v>
       </c>
       <c r="B21">
-        <v>2.2999999999999998</v>
+        <v>2.4</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E21" t="s">
         <v>17</v>
@@ -4219,33 +4219,33 @@
         <v>2</v>
       </c>
       <c r="B22">
-        <v>2.4</v>
+        <v>2.5</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D22" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E22" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2</v>
       </c>
-      <c r="B23">
-        <v>2.5</v>
+      <c r="B23" t="s">
+        <v>44</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D23" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E23" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -4256,10 +4256,10 @@
         <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E24" t="s">
         <v>7</v>
@@ -4270,13 +4270,13 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D25" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E25" t="s">
         <v>7</v>
@@ -4287,33 +4287,33 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D26" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E26" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>2</v>
-      </c>
-      <c r="B27" t="s">
-        <v>52</v>
+        <v>3</v>
+      </c>
+      <c r="B27">
+        <v>3.1</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D27" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E27" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -4324,13 +4324,13 @@
         <v>3.1</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D28" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E28" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -4338,13 +4338,13 @@
         <v>3</v>
       </c>
       <c r="B29">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="C29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D29" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E29" t="s">
         <v>7</v>
@@ -4355,13 +4355,13 @@
         <v>3</v>
       </c>
       <c r="B30">
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="C30" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D30" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E30" t="s">
         <v>7</v>
@@ -4375,10 +4375,10 @@
         <v>3.3</v>
       </c>
       <c r="C31" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D31" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E31" t="s">
         <v>7</v>
@@ -4392,10 +4392,10 @@
         <v>3.3</v>
       </c>
       <c r="C32" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D32" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E32" t="s">
         <v>7</v>
@@ -4409,13 +4409,13 @@
         <v>3.3</v>
       </c>
       <c r="C33" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D33" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E33" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -4423,13 +4423,13 @@
         <v>3</v>
       </c>
       <c r="B34">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="C34" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D34" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E34" t="s">
         <v>12</v>
@@ -4443,10 +4443,10 @@
         <v>3.4</v>
       </c>
       <c r="C35" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D35" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E35" t="s">
         <v>12</v>
@@ -4457,16 +4457,16 @@
         <v>3</v>
       </c>
       <c r="B36">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="C36" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D36" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E36" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -4477,13 +4477,13 @@
         <v>3.5</v>
       </c>
       <c r="C37" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D37" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E37" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -4491,13 +4491,13 @@
         <v>3</v>
       </c>
       <c r="B38">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="C38" t="s">
-        <v>76</v>
+        <v>637</v>
       </c>
       <c r="D38" t="s">
-        <v>77</v>
+        <v>638</v>
       </c>
       <c r="E38" t="s">
         <v>7</v>
@@ -4508,13 +4508,13 @@
         <v>3</v>
       </c>
       <c r="B39">
-        <v>3.6</v>
+        <v>3.7</v>
       </c>
       <c r="C39" t="s">
-        <v>637</v>
+        <v>78</v>
       </c>
       <c r="D39" t="s">
-        <v>638</v>
+        <v>79</v>
       </c>
       <c r="E39" t="s">
         <v>7</v>
@@ -4528,10 +4528,10 @@
         <v>3.7</v>
       </c>
       <c r="C40" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D40" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E40" t="s">
         <v>7</v>
@@ -4542,16 +4542,16 @@
         <v>3</v>
       </c>
       <c r="B41">
-        <v>3.7</v>
+        <v>3.8</v>
       </c>
       <c r="C41" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D41" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E41" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -4559,16 +4559,16 @@
         <v>3</v>
       </c>
       <c r="B42">
-        <v>3.8</v>
+        <v>3.9</v>
       </c>
       <c r="C42" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D42" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E42" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -4579,30 +4579,30 @@
         <v>3.9</v>
       </c>
       <c r="C43" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D43" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E43" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>3</v>
       </c>
-      <c r="B44">
-        <v>3.9</v>
+      <c r="B44" t="s">
+        <v>88</v>
       </c>
       <c r="C44" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D44" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E44" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -4610,17 +4610,15 @@
         <v>3</v>
       </c>
       <c r="B45" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C45" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D45" t="s">
-        <v>90</v>
-      </c>
-      <c r="E45" t="s">
-        <v>7</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="E45"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
@@ -4630,25 +4628,27 @@
         <v>91</v>
       </c>
       <c r="C46" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D46" t="s">
-        <v>93</v>
-      </c>
-      <c r="E46"/>
+        <v>95</v>
+      </c>
+      <c r="E46" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>3</v>
       </c>
       <c r="B47" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C47" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D47" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E47" t="s">
         <v>7</v>
@@ -4659,33 +4659,33 @@
         <v>3</v>
       </c>
       <c r="B48" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C48" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D48" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E48" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>3</v>
-      </c>
-      <c r="B49" t="s">
-        <v>99</v>
+        <v>4</v>
+      </c>
+      <c r="B49">
+        <v>4.0999999999999996</v>
       </c>
       <c r="C49" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D49" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E49" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -4693,16 +4693,16 @@
         <v>4</v>
       </c>
       <c r="B50">
-        <v>4.0999999999999996</v>
+        <v>4.2</v>
       </c>
       <c r="C50" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D50" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E50" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -4713,13 +4713,13 @@
         <v>4.2</v>
       </c>
       <c r="C51" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D51" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E51" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -4727,16 +4727,16 @@
         <v>4</v>
       </c>
       <c r="B52">
-        <v>4.2</v>
+        <v>4.3</v>
       </c>
       <c r="C52" t="s">
-        <v>106</v>
+        <v>639</v>
       </c>
       <c r="D52" t="s">
-        <v>107</v>
+        <v>640</v>
       </c>
       <c r="E52" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -4744,13 +4744,13 @@
         <v>4</v>
       </c>
       <c r="B53">
-        <v>4.3</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C53" t="s">
-        <v>639</v>
+        <v>108</v>
       </c>
       <c r="D53" t="s">
-        <v>640</v>
+        <v>109</v>
       </c>
       <c r="E53" t="s">
         <v>12</v>
@@ -4761,16 +4761,16 @@
         <v>4</v>
       </c>
       <c r="B54">
-        <v>4.4000000000000004</v>
+        <v>4.5</v>
       </c>
       <c r="C54" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D54" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E54" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -4778,13 +4778,13 @@
         <v>4</v>
       </c>
       <c r="B55">
-        <v>4.5</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C55" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D55" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E55" t="s">
         <v>7</v>
@@ -4795,13 +4795,13 @@
         <v>4</v>
       </c>
       <c r="B56">
-        <v>4.5999999999999996</v>
+        <v>4.7</v>
       </c>
       <c r="C56" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D56" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E56" t="s">
         <v>7</v>
@@ -4811,14 +4811,14 @@
       <c r="A57">
         <v>4</v>
       </c>
-      <c r="B57">
-        <v>4.7</v>
+      <c r="B57" t="s">
+        <v>116</v>
       </c>
       <c r="C57" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D57" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E57" t="s">
         <v>7</v>
@@ -4829,13 +4829,13 @@
         <v>4</v>
       </c>
       <c r="B58" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C58" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D58" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E58" t="s">
         <v>7</v>
@@ -4843,19 +4843,19 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>4</v>
-      </c>
-      <c r="B59" t="s">
-        <v>119</v>
+        <v>5</v>
+      </c>
+      <c r="B59">
+        <v>5.0999999999999996</v>
       </c>
       <c r="C59" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D59" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E59" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -4863,16 +4863,16 @@
         <v>5</v>
       </c>
       <c r="B60">
-        <v>5.0999999999999996</v>
+        <v>5.2</v>
       </c>
       <c r="C60" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D60" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E60" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -4883,10 +4883,10 @@
         <v>5.2</v>
       </c>
       <c r="C61" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D61" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E61" t="s">
         <v>12</v>
@@ -4897,16 +4897,16 @@
         <v>5</v>
       </c>
       <c r="B62">
-        <v>5.2</v>
+        <v>5.3</v>
       </c>
       <c r="C62" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D62" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E62" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -4917,10 +4917,10 @@
         <v>5.3</v>
       </c>
       <c r="C63" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D63" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E63" t="s">
         <v>7</v>
@@ -4931,16 +4931,16 @@
         <v>5</v>
       </c>
       <c r="B64">
-        <v>5.3</v>
+        <v>5.4</v>
       </c>
       <c r="C64" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D64" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E64" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -4948,16 +4948,16 @@
         <v>5</v>
       </c>
       <c r="B65">
-        <v>5.4</v>
+        <v>5.5</v>
       </c>
       <c r="C65" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D65" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E65" t="s">
-        <v>12</v>
+        <v>136</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -4968,13 +4968,13 @@
         <v>5.5</v>
       </c>
       <c r="C66" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D66" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E66" t="s">
-        <v>136</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -4982,30 +4982,30 @@
         <v>5</v>
       </c>
       <c r="B67">
-        <v>5.5</v>
+        <v>5.6</v>
       </c>
       <c r="C67" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D67" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E67" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>5</v>
       </c>
-      <c r="B68">
-        <v>5.6</v>
+      <c r="B68" t="s">
+        <v>141</v>
       </c>
       <c r="C68" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D68" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="E68" t="s">
         <v>17</v>
@@ -5019,10 +5019,10 @@
         <v>141</v>
       </c>
       <c r="C69" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D69" t="s">
-        <v>143</v>
+        <v>641</v>
       </c>
       <c r="E69" t="s">
         <v>17</v>
@@ -5033,16 +5033,16 @@
         <v>5</v>
       </c>
       <c r="B70" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C70" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D70" t="s">
-        <v>641</v>
+        <v>147</v>
       </c>
       <c r="E70" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -5050,33 +5050,33 @@
         <v>5</v>
       </c>
       <c r="B71" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C71" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D71" t="s">
-        <v>147</v>
+        <v>642</v>
       </c>
       <c r="E71" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>5</v>
-      </c>
-      <c r="B72" t="s">
-        <v>148</v>
+        <v>6</v>
+      </c>
+      <c r="B72">
+        <v>6.1</v>
       </c>
       <c r="C72" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D72" t="s">
-        <v>642</v>
+        <v>151</v>
       </c>
       <c r="E72" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -5084,13 +5084,13 @@
         <v>6</v>
       </c>
       <c r="B73">
-        <v>6.1</v>
+        <v>6.3</v>
       </c>
       <c r="C73" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D73" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E73" t="s">
         <v>7</v>
@@ -5101,16 +5101,16 @@
         <v>6</v>
       </c>
       <c r="B74">
-        <v>6.3</v>
+        <v>6.4</v>
       </c>
       <c r="C74" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D74" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E74" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
@@ -5121,13 +5121,13 @@
         <v>6.4</v>
       </c>
       <c r="C75" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D75" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E75" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
@@ -5135,33 +5135,33 @@
         <v>6</v>
       </c>
       <c r="B76">
-        <v>6.4</v>
+        <v>6.5</v>
       </c>
       <c r="C76" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D76" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E76" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>6</v>
       </c>
-      <c r="B77">
-        <v>6.5</v>
+      <c r="B77" t="s">
+        <v>160</v>
       </c>
       <c r="C77" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D77" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="E77" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -5175,7 +5175,7 @@
         <v>161</v>
       </c>
       <c r="D78" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E78" t="s">
         <v>7</v>
@@ -5183,16 +5183,16 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>6</v>
-      </c>
-      <c r="B79" t="s">
-        <v>160</v>
+        <v>7</v>
+      </c>
+      <c r="B79">
+        <v>7.1</v>
       </c>
       <c r="C79" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D79" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E79" t="s">
         <v>7</v>
@@ -5203,13 +5203,13 @@
         <v>7</v>
       </c>
       <c r="B80">
-        <v>7.1</v>
+        <v>7.2</v>
       </c>
       <c r="C80" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D80" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E80" t="s">
         <v>7</v>
@@ -5220,13 +5220,13 @@
         <v>7</v>
       </c>
       <c r="B81">
-        <v>7.2</v>
+        <v>7.3</v>
       </c>
       <c r="C81" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D81" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E81" t="s">
         <v>7</v>
@@ -5236,34 +5236,34 @@
       <c r="A82">
         <v>7</v>
       </c>
-      <c r="B82">
-        <v>7.3</v>
+      <c r="B82" t="s">
+        <v>170</v>
       </c>
       <c r="C82" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D82" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="E82" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>7</v>
-      </c>
-      <c r="B83" t="s">
-        <v>170</v>
+        <v>8</v>
+      </c>
+      <c r="B83">
+        <v>8.1</v>
       </c>
       <c r="C83" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D83" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E83" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
@@ -5271,13 +5271,13 @@
         <v>8</v>
       </c>
       <c r="B84">
-        <v>8.1</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C84" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D84" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E84" t="s">
         <v>7</v>
@@ -5288,16 +5288,16 @@
         <v>8</v>
       </c>
       <c r="B85">
-        <v>8.1999999999999993</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="C85" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D85" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E85" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -5305,13 +5305,13 @@
         <v>8</v>
       </c>
       <c r="B86">
-        <v>8.3000000000000007</v>
+        <v>8.4</v>
       </c>
       <c r="C86" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D86" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E86" t="s">
         <v>12</v>
@@ -5325,13 +5325,13 @@
         <v>8.4</v>
       </c>
       <c r="C87" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D87" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E87" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -5339,13 +5339,13 @@
         <v>8</v>
       </c>
       <c r="B88">
-        <v>8.4</v>
+        <v>8.5</v>
       </c>
       <c r="C88" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D88" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E88" t="s">
         <v>7</v>
@@ -5359,10 +5359,10 @@
         <v>8.5</v>
       </c>
       <c r="C89" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D89" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E89" t="s">
         <v>7</v>
@@ -5373,13 +5373,13 @@
         <v>8</v>
       </c>
       <c r="B90">
-        <v>8.5</v>
+        <v>8.6</v>
       </c>
       <c r="C90" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D90" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E90" t="s">
         <v>7</v>
@@ -5390,13 +5390,13 @@
         <v>8</v>
       </c>
       <c r="B91">
-        <v>8.6</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="C91" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D91" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E91" t="s">
         <v>7</v>
@@ -5407,13 +5407,13 @@
         <v>8</v>
       </c>
       <c r="B92">
-        <v>8.6999999999999993</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="C92" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D92" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E92" t="s">
         <v>7</v>
@@ -5424,16 +5424,16 @@
         <v>8</v>
       </c>
       <c r="B93">
-        <v>8.8000000000000007</v>
+        <v>8.9</v>
       </c>
       <c r="C93" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D93" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E93" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -5444,10 +5444,10 @@
         <v>8.9</v>
       </c>
       <c r="C94" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D94" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E94" t="s">
         <v>12</v>
@@ -5458,16 +5458,16 @@
         <v>8</v>
       </c>
       <c r="B95">
-        <v>8.9</v>
+        <v>8.1</v>
       </c>
       <c r="C95" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D95" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E95" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -5478,10 +5478,10 @@
         <v>8.1</v>
       </c>
       <c r="C96" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D96" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E96" t="s">
         <v>7</v>
@@ -5491,14 +5491,14 @@
       <c r="A97">
         <v>8</v>
       </c>
-      <c r="B97">
-        <v>8.1</v>
+      <c r="B97" t="s">
+        <v>201</v>
       </c>
       <c r="C97" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D97" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="E97" t="s">
         <v>7</v>
@@ -5509,30 +5509,30 @@
         <v>8</v>
       </c>
       <c r="B98" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C98" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D98" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E98" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99">
-        <v>8</v>
-      </c>
-      <c r="B99" t="s">
-        <v>204</v>
+        <v>9</v>
+      </c>
+      <c r="B99">
+        <v>9.1</v>
       </c>
       <c r="C99" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D99" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="E99" t="s">
         <v>17</v>
@@ -5546,13 +5546,13 @@
         <v>9.1</v>
       </c>
       <c r="C100" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D100" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="E100" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
@@ -5560,13 +5560,13 @@
         <v>9</v>
       </c>
       <c r="B101">
-        <v>9.1</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="C101" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D101" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E101" t="s">
         <v>7</v>
@@ -5577,16 +5577,16 @@
         <v>9</v>
       </c>
       <c r="B102">
-        <v>9.1999999999999993</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="C102" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D102" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E102" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
@@ -5597,10 +5597,10 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="C103" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D103" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="E103" t="s">
         <v>17</v>
@@ -5611,16 +5611,16 @@
         <v>9</v>
       </c>
       <c r="B104">
-        <v>9.3000000000000007</v>
+        <v>9.5</v>
       </c>
       <c r="C104" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D104" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="E104" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
@@ -5631,10 +5631,10 @@
         <v>9.5</v>
       </c>
       <c r="C105" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D105" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E105" t="s">
         <v>7</v>
@@ -5644,14 +5644,14 @@
       <c r="A106">
         <v>9</v>
       </c>
-      <c r="B106">
-        <v>9.5</v>
+      <c r="B106" t="s">
+        <v>221</v>
       </c>
       <c r="C106" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D106" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E106" t="s">
         <v>7</v>
@@ -5662,33 +5662,33 @@
         <v>9</v>
       </c>
       <c r="B107" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C107" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D107" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="E107" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108">
-        <v>9</v>
-      </c>
-      <c r="B108" t="s">
-        <v>224</v>
+        <v>10</v>
+      </c>
+      <c r="B108">
+        <v>10.1</v>
       </c>
       <c r="C108" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D108" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E108" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
@@ -5696,16 +5696,16 @@
         <v>10</v>
       </c>
       <c r="B109">
-        <v>10.1</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="C109" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D109" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="E109" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
@@ -5713,13 +5713,13 @@
         <v>10</v>
       </c>
       <c r="B110">
-        <v>10.199999999999999</v>
+        <v>10.3</v>
       </c>
       <c r="C110" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D110" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="E110" t="s">
         <v>17</v>
@@ -5730,16 +5730,16 @@
         <v>10</v>
       </c>
       <c r="B111">
-        <v>10.3</v>
+        <v>10.4</v>
       </c>
       <c r="C111" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D111" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="E111" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
@@ -5747,16 +5747,16 @@
         <v>10</v>
       </c>
       <c r="B112">
-        <v>10.4</v>
+        <v>10.5</v>
       </c>
       <c r="C112" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D112" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E112" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
@@ -5764,16 +5764,16 @@
         <v>10</v>
       </c>
       <c r="B113">
-        <v>10.5</v>
+        <v>10.6</v>
       </c>
       <c r="C113" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D113" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="E113" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
@@ -5781,33 +5781,33 @@
         <v>10</v>
       </c>
       <c r="B114">
-        <v>10.6</v>
+        <v>10.7</v>
       </c>
       <c r="C114" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D114" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="E114" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>10</v>
       </c>
-      <c r="B115">
-        <v>10.7</v>
+      <c r="B115" t="s">
+        <v>241</v>
       </c>
       <c r="C115" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D115" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="E115" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
@@ -5815,33 +5815,33 @@
         <v>10</v>
       </c>
       <c r="B116" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="C116" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="D116" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="E116" t="s">
-        <v>7</v>
+        <v>247</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117">
-        <v>10</v>
-      </c>
-      <c r="B117" t="s">
-        <v>244</v>
+        <v>11</v>
+      </c>
+      <c r="B117">
+        <v>11.1</v>
       </c>
       <c r="C117" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="D117" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="E117" t="s">
-        <v>247</v>
+        <v>7</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
@@ -5849,16 +5849,16 @@
         <v>11</v>
       </c>
       <c r="B118">
-        <v>11.1</v>
+        <v>11.3</v>
       </c>
       <c r="C118" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="D118" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="E118" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -5869,13 +5869,13 @@
         <v>11.3</v>
       </c>
       <c r="C119" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D119" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="E119" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
@@ -5883,13 +5883,13 @@
         <v>11</v>
       </c>
       <c r="B120">
-        <v>11.3</v>
+        <v>11.4</v>
       </c>
       <c r="C120" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D120" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E120" t="s">
         <v>17</v>
@@ -5900,16 +5900,16 @@
         <v>11</v>
       </c>
       <c r="B121">
-        <v>11.4</v>
+        <v>11.5</v>
       </c>
       <c r="C121" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D121" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E121" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
@@ -5917,16 +5917,16 @@
         <v>11</v>
       </c>
       <c r="B122">
-        <v>11.5</v>
+        <v>11.6</v>
       </c>
       <c r="C122" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D122" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E122" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
@@ -5934,16 +5934,16 @@
         <v>11</v>
       </c>
       <c r="B123">
-        <v>11.6</v>
+        <v>11.7</v>
       </c>
       <c r="C123" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="D123" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="E123" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
@@ -5954,27 +5954,27 @@
         <v>11.7</v>
       </c>
       <c r="C124" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D124" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="E124" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>11</v>
       </c>
-      <c r="B125">
-        <v>11.7</v>
+      <c r="B125" t="s">
+        <v>264</v>
       </c>
       <c r="C125" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D125" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="E125" t="s">
         <v>17</v>
@@ -5982,19 +5982,19 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126">
-        <v>11</v>
-      </c>
-      <c r="B126" t="s">
-        <v>264</v>
+        <v>12</v>
+      </c>
+      <c r="B126">
+        <v>12.2</v>
       </c>
       <c r="C126" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D126" t="s">
-        <v>266</v>
+        <v>182</v>
       </c>
       <c r="E126" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
@@ -6002,16 +6002,16 @@
         <v>12</v>
       </c>
       <c r="B127">
-        <v>12.2</v>
+        <v>12.3</v>
       </c>
       <c r="C127" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D127" t="s">
-        <v>182</v>
+        <v>269</v>
       </c>
       <c r="E127" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
@@ -6019,16 +6019,16 @@
         <v>12</v>
       </c>
       <c r="B128">
-        <v>12.3</v>
+        <v>12.4</v>
       </c>
       <c r="C128" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D128" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="E128" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
@@ -6039,13 +6039,13 @@
         <v>12.4</v>
       </c>
       <c r="C129" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D129" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="E129" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
@@ -6053,16 +6053,16 @@
         <v>12</v>
       </c>
       <c r="B130">
-        <v>12.4</v>
+        <v>12.6</v>
       </c>
       <c r="C130" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D130" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="E130" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
@@ -6070,16 +6070,16 @@
         <v>12</v>
       </c>
       <c r="B131">
-        <v>12.6</v>
+        <v>12.7</v>
       </c>
       <c r="C131" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D131" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="E131" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
@@ -6087,33 +6087,33 @@
         <v>12</v>
       </c>
       <c r="B132">
-        <v>12.7</v>
+        <v>12.8</v>
       </c>
       <c r="C132" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D132" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="E132" t="s">
-        <v>17</v>
+        <v>280</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>12</v>
       </c>
-      <c r="B133">
-        <v>12.8</v>
+      <c r="B133" t="s">
+        <v>281</v>
       </c>
       <c r="C133" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="D133" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="E133" t="s">
-        <v>280</v>
+        <v>12</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
@@ -6121,33 +6121,33 @@
         <v>12</v>
       </c>
       <c r="B134" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="C134" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="D134" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="E134" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135">
-        <v>12</v>
-      </c>
-      <c r="B135" t="s">
-        <v>284</v>
+        <v>13</v>
+      </c>
+      <c r="B135">
+        <v>13.1</v>
       </c>
       <c r="C135" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="D135" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="E135" t="s">
-        <v>17</v>
+        <v>289</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
@@ -6155,16 +6155,16 @@
         <v>13</v>
       </c>
       <c r="B136">
-        <v>13.1</v>
+        <v>13.2</v>
       </c>
       <c r="C136" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="D136" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="E136" t="s">
-        <v>289</v>
+        <v>17</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
@@ -6172,13 +6172,13 @@
         <v>13</v>
       </c>
       <c r="B137">
-        <v>13.2</v>
+        <v>13.3</v>
       </c>
       <c r="C137" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="D137" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="E137" t="s">
         <v>17</v>
@@ -6192,10 +6192,10 @@
         <v>13.3</v>
       </c>
       <c r="C138" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D138" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="E138" t="s">
         <v>17</v>
@@ -6205,14 +6205,14 @@
       <c r="A139">
         <v>13</v>
       </c>
-      <c r="B139">
-        <v>13.3</v>
+      <c r="B139" t="s">
+        <v>296</v>
       </c>
       <c r="C139" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="D139" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="E139" t="s">
         <v>17</v>
@@ -6223,45 +6223,45 @@
         <v>13</v>
       </c>
       <c r="B140" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="C140" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="D140" t="s">
-        <v>298</v>
-      </c>
-      <c r="E140" t="s">
-        <v>17</v>
-      </c>
+        <v>301</v>
+      </c>
+      <c r="E140"/>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141">
-        <v>13</v>
-      </c>
-      <c r="B141" t="s">
-        <v>299</v>
+        <v>14</v>
+      </c>
+      <c r="B141">
+        <v>14.1</v>
       </c>
       <c r="C141" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="D141" t="s">
-        <v>301</v>
-      </c>
-      <c r="E141"/>
+        <v>303</v>
+      </c>
+      <c r="E141" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>14</v>
       </c>
       <c r="B142">
-        <v>14.1</v>
+        <v>14.2</v>
       </c>
       <c r="C142" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="D142" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="E142" t="s">
         <v>17</v>
@@ -6272,16 +6272,16 @@
         <v>14</v>
       </c>
       <c r="B143">
-        <v>14.2</v>
+        <v>14.4</v>
       </c>
       <c r="C143" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="D143" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="E143" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
@@ -6289,13 +6289,13 @@
         <v>14</v>
       </c>
       <c r="B144">
-        <v>14.4</v>
+        <v>14.5</v>
       </c>
       <c r="C144" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="D144" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="E144" t="s">
         <v>7</v>
@@ -6306,16 +6306,16 @@
         <v>14</v>
       </c>
       <c r="B145">
-        <v>14.5</v>
+        <v>14.6</v>
       </c>
       <c r="C145" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="D145" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="E145" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
@@ -6323,33 +6323,33 @@
         <v>14</v>
       </c>
       <c r="B146">
-        <v>14.6</v>
+        <v>14.7</v>
       </c>
       <c r="C146" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D146" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="E146" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>14</v>
       </c>
-      <c r="B147">
-        <v>14.7</v>
+      <c r="B147" t="s">
+        <v>314</v>
       </c>
       <c r="C147" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="D147" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E147" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
@@ -6357,13 +6357,13 @@
         <v>14</v>
       </c>
       <c r="B148" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="C148" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="D148" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="E148" t="s">
         <v>17</v>
@@ -6371,19 +6371,19 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149">
-        <v>14</v>
-      </c>
-      <c r="B149" t="s">
-        <v>317</v>
+        <v>15</v>
+      </c>
+      <c r="B149">
+        <v>15.1</v>
       </c>
       <c r="C149" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D149" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="E149" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
@@ -6394,10 +6394,10 @@
         <v>15.1</v>
       </c>
       <c r="C150" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D150" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="E150" t="s">
         <v>7</v>
@@ -6408,16 +6408,16 @@
         <v>15</v>
       </c>
       <c r="B151">
-        <v>15.1</v>
+        <v>15.2</v>
       </c>
       <c r="C151" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="D151" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="E151" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
@@ -6425,16 +6425,16 @@
         <v>15</v>
       </c>
       <c r="B152">
-        <v>15.2</v>
+        <v>15.4</v>
       </c>
       <c r="C152" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="D152" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="E152" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
@@ -6445,13 +6445,13 @@
         <v>15.4</v>
       </c>
       <c r="C153" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="D153" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="E153" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
@@ -6459,16 +6459,16 @@
         <v>15</v>
       </c>
       <c r="B154">
-        <v>15.4</v>
+        <v>15.5</v>
       </c>
       <c r="C154" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D154" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="E154" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
@@ -6476,16 +6476,16 @@
         <v>15</v>
       </c>
       <c r="B155">
-        <v>15.5</v>
+        <v>15.6</v>
       </c>
       <c r="C155" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="D155" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="E155" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
@@ -6493,16 +6493,16 @@
         <v>15</v>
       </c>
       <c r="B156">
-        <v>15.6</v>
+        <v>15.7</v>
       </c>
       <c r="C156" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="D156" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="E156" t="s">
-        <v>17</v>
+        <v>336</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
@@ -6510,16 +6510,16 @@
         <v>15</v>
       </c>
       <c r="B157">
-        <v>15.7</v>
+        <v>15.8</v>
       </c>
       <c r="C157" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="D157" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="E157" t="s">
-        <v>336</v>
+        <v>17</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
@@ -6527,13 +6527,13 @@
         <v>15</v>
       </c>
       <c r="B158">
-        <v>15.8</v>
+        <v>15.9</v>
       </c>
       <c r="C158" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D158" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="E158" t="s">
         <v>17</v>
@@ -6543,17 +6543,17 @@
       <c r="A159">
         <v>15</v>
       </c>
-      <c r="B159">
-        <v>15.9</v>
+      <c r="B159" t="s">
+        <v>341</v>
       </c>
       <c r="C159" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="D159" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="E159" t="s">
-        <v>17</v>
+        <v>344</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
@@ -6561,32 +6561,32 @@
         <v>15</v>
       </c>
       <c r="B160" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="C160" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="D160" t="s">
-        <v>343</v>
-      </c>
-      <c r="E160" t="s">
-        <v>344</v>
-      </c>
+        <v>335</v>
+      </c>
+      <c r="E160"/>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161">
-        <v>15</v>
-      </c>
-      <c r="B161" t="s">
-        <v>345</v>
+        <v>16</v>
+      </c>
+      <c r="B161">
+        <v>16.100000000000001</v>
       </c>
       <c r="C161" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D161" t="s">
-        <v>335</v>
-      </c>
-      <c r="E161"/>
+        <v>348</v>
+      </c>
+      <c r="E161" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162">
@@ -6596,13 +6596,13 @@
         <v>16.100000000000001</v>
       </c>
       <c r="C162" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="D162" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="E162" t="s">
-        <v>7</v>
+        <v>351</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
@@ -6613,13 +6613,13 @@
         <v>16.100000000000001</v>
       </c>
       <c r="C163" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="D163" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="E163" t="s">
-        <v>351</v>
+        <v>12</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
@@ -6630,10 +6630,10 @@
         <v>16.100000000000001</v>
       </c>
       <c r="C164" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="D164" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="E164" t="s">
         <v>12</v>
@@ -6644,16 +6644,16 @@
         <v>16</v>
       </c>
       <c r="B165">
-        <v>16.100000000000001</v>
+        <v>16.2</v>
       </c>
       <c r="C165" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="D165" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E165" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
@@ -6664,13 +6664,13 @@
         <v>16.2</v>
       </c>
       <c r="C166" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="D166" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="E166" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
@@ -6678,13 +6678,13 @@
         <v>16</v>
       </c>
       <c r="B167">
-        <v>16.2</v>
+        <v>16.3</v>
       </c>
       <c r="C167" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="D167" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="E167" t="s">
         <v>12</v>
@@ -6698,13 +6698,13 @@
         <v>16.3</v>
       </c>
       <c r="C168" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="D168" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="E168" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
@@ -6712,16 +6712,16 @@
         <v>16</v>
       </c>
       <c r="B169">
-        <v>16.3</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="C169" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="D169" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="E169" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
@@ -6729,13 +6729,13 @@
         <v>16</v>
       </c>
       <c r="B170">
-        <v>16.399999999999999</v>
+        <v>16.5</v>
       </c>
       <c r="C170" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="D170" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="E170" t="s">
         <v>12</v>
@@ -6749,13 +6749,13 @@
         <v>16.5</v>
       </c>
       <c r="C171" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="D171" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="E171" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
@@ -6763,16 +6763,16 @@
         <v>16</v>
       </c>
       <c r="B172">
-        <v>16.5</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="C172" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="D172" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="E172" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
@@ -6780,16 +6780,16 @@
         <v>16</v>
       </c>
       <c r="B173">
-        <v>16.600000000000001</v>
+        <v>16.7</v>
       </c>
       <c r="C173" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="D173" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="E173" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
@@ -6800,10 +6800,10 @@
         <v>16.7</v>
       </c>
       <c r="C174" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="D174" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="E174" t="s">
         <v>17</v>
@@ -6814,16 +6814,16 @@
         <v>16</v>
       </c>
       <c r="B175">
-        <v>16.7</v>
+        <v>16.8</v>
       </c>
       <c r="C175" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="D175" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="E175" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
@@ -6831,13 +6831,13 @@
         <v>16</v>
       </c>
       <c r="B176">
-        <v>16.8</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="C176" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="D176" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="E176" t="s">
         <v>7</v>
@@ -6848,16 +6848,16 @@
         <v>16</v>
       </c>
       <c r="B177">
-        <v>16.899999999999999</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="C177" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="D177" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="E177" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
@@ -6868,30 +6868,30 @@
         <v>16.100000000000001</v>
       </c>
       <c r="C178" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="D178" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="E178" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>16</v>
       </c>
-      <c r="B179">
-        <v>16.100000000000001</v>
+      <c r="B179" t="s">
+        <v>384</v>
       </c>
       <c r="C179" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="D179" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="E179" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
@@ -6899,33 +6899,33 @@
         <v>16</v>
       </c>
       <c r="B180" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="C180" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="D180" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="E180" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181">
-        <v>16</v>
-      </c>
-      <c r="B181" t="s">
-        <v>387</v>
+        <v>17</v>
+      </c>
+      <c r="B181">
+        <v>17.100000000000001</v>
       </c>
       <c r="C181" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="D181" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="E181" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
@@ -6936,10 +6936,10 @@
         <v>17.100000000000001</v>
       </c>
       <c r="C182" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="D182" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="E182" t="s">
         <v>7</v>
@@ -6950,13 +6950,13 @@
         <v>17</v>
       </c>
       <c r="B183">
-        <v>17.100000000000001</v>
+        <v>17.2</v>
       </c>
       <c r="C183" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="D183" t="s">
-        <v>393</v>
+        <v>643</v>
       </c>
       <c r="E183" t="s">
         <v>7</v>
@@ -6967,13 +6967,13 @@
         <v>17</v>
       </c>
       <c r="B184">
-        <v>17.2</v>
+        <v>17.3</v>
       </c>
       <c r="C184" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D184" t="s">
-        <v>643</v>
+        <v>396</v>
       </c>
       <c r="E184" t="s">
         <v>7</v>
@@ -6987,10 +6987,10 @@
         <v>17.3</v>
       </c>
       <c r="C185" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="D185" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="E185" t="s">
         <v>7</v>
@@ -7001,13 +7001,13 @@
         <v>17</v>
       </c>
       <c r="B186">
-        <v>17.3</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="C186" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="D186" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="E186" t="s">
         <v>7</v>
@@ -7018,30 +7018,28 @@
         <v>17</v>
       </c>
       <c r="B187">
-        <v>17.399999999999999</v>
+        <v>17.5</v>
       </c>
       <c r="C187" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="D187" t="s">
-        <v>400</v>
-      </c>
-      <c r="E187" t="s">
-        <v>7</v>
-      </c>
+        <v>402</v>
+      </c>
+      <c r="E187"/>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>17</v>
       </c>
       <c r="B188">
-        <v>17.5</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="C188" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="D188" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="E188"/>
     </row>
@@ -7053,28 +7051,30 @@
         <v>17.600000000000001</v>
       </c>
       <c r="C189" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="D189" t="s">
-        <v>404</v>
-      </c>
-      <c r="E189"/>
+        <v>406</v>
+      </c>
+      <c r="E189" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>17</v>
       </c>
       <c r="B190">
-        <v>17.600000000000001</v>
+        <v>17.7</v>
       </c>
       <c r="C190" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D190" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="E190" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
@@ -7082,16 +7082,16 @@
         <v>17</v>
       </c>
       <c r="B191">
-        <v>17.7</v>
+        <v>17.8</v>
       </c>
       <c r="C191" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="D191" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="E191" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
@@ -7099,13 +7099,13 @@
         <v>17</v>
       </c>
       <c r="B192">
-        <v>17.8</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="C192" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="D192" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="E192" t="s">
         <v>7</v>
@@ -7116,13 +7116,13 @@
         <v>17</v>
       </c>
       <c r="B193">
-        <v>17.899999999999999</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="C193" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="D193" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="E193" t="s">
         <v>7</v>
@@ -7133,13 +7133,13 @@
         <v>17</v>
       </c>
       <c r="B194">
-        <v>17.100000000000001</v>
+        <v>17.11</v>
       </c>
       <c r="C194" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="D194" t="s">
-        <v>414</v>
+        <v>644</v>
       </c>
       <c r="E194" t="s">
         <v>7</v>
@@ -7150,13 +7150,13 @@
         <v>17</v>
       </c>
       <c r="B195">
-        <v>17.11</v>
+        <v>17.12</v>
       </c>
       <c r="C195" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D195" t="s">
-        <v>644</v>
+        <v>417</v>
       </c>
       <c r="E195" t="s">
         <v>7</v>
@@ -7167,48 +7167,48 @@
         <v>17</v>
       </c>
       <c r="B196">
-        <v>17.12</v>
+        <v>17.13</v>
       </c>
       <c r="C196" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="D196" t="s">
-        <v>417</v>
-      </c>
-      <c r="E196" t="s">
-        <v>7</v>
-      </c>
+        <v>419</v>
+      </c>
+      <c r="E196"/>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>17</v>
       </c>
       <c r="B197">
-        <v>17.13</v>
+        <v>17.14</v>
       </c>
       <c r="C197" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="D197" t="s">
-        <v>419</v>
-      </c>
-      <c r="E197"/>
+        <v>421</v>
+      </c>
+      <c r="E197" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>17</v>
       </c>
       <c r="B198">
-        <v>17.14</v>
+        <v>17.149999999999999</v>
       </c>
       <c r="C198" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="D198" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="E198" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
@@ -7216,13 +7216,13 @@
         <v>17</v>
       </c>
       <c r="B199">
-        <v>17.149999999999999</v>
+        <v>17.16</v>
       </c>
       <c r="C199" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="D199" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="E199" t="s">
         <v>7</v>
@@ -7233,16 +7233,16 @@
         <v>17</v>
       </c>
       <c r="B200">
-        <v>17.16</v>
+        <v>17.170000000000002</v>
       </c>
       <c r="C200" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="D200" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="E200" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
@@ -7250,13 +7250,13 @@
         <v>17</v>
       </c>
       <c r="B201">
-        <v>17.170000000000002</v>
+        <v>17.18</v>
       </c>
       <c r="C201" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="D201" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="E201" t="s">
         <v>17</v>
@@ -7270,10 +7270,10 @@
         <v>17.18</v>
       </c>
       <c r="C202" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="D202" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="E202" t="s">
         <v>17</v>
@@ -7287,13 +7287,13 @@
         <v>17.18</v>
       </c>
       <c r="C203" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="D203" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="E203" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
@@ -7301,32 +7301,15 @@
         <v>17</v>
       </c>
       <c r="B204">
-        <v>17.18</v>
+        <v>17.190000000000001</v>
       </c>
       <c r="C204" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="D204" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="E204" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A205">
-        <v>17</v>
-      </c>
-      <c r="B205">
-        <v>17.190000000000001</v>
-      </c>
-      <c r="C205" t="s">
-        <v>434</v>
-      </c>
-      <c r="D205" t="s">
-        <v>435</v>
-      </c>
-      <c r="E205" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>